<commit_message>
updated matlab files with new calculations. Added figures to excel sheet
</commit_message>
<xml_diff>
--- a/Resistance and results table.xlsx
+++ b/Resistance and results table.xlsx
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>mdxtech</author>
+  </authors>
+  <commentList>
+    <comment ref="O7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mdxtech:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Measured value</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Measured Current (A)</t>
   </si>
@@ -90,12 +124,102 @@
   <si>
     <t>V/(As)</t>
   </si>
+  <si>
+    <t>Ieq</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Peak Second Peak Time</t>
+  </si>
+  <si>
+    <t>First Peak Time</t>
+  </si>
+  <si>
+    <t>Peak Time Difference</t>
+  </si>
+  <si>
+    <t>Wd</t>
+  </si>
+  <si>
+    <t>Rad/s</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>mh</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Propeller mass</t>
+  </si>
+  <si>
+    <t>VTOL body mass</t>
+  </si>
+  <si>
+    <t>Length from pivot to propeller center</t>
+  </si>
+  <si>
+    <t>length from pivot to center of counter-weight</t>
+  </si>
+  <si>
+    <t>Total length of helicopter body</t>
+  </si>
+  <si>
+    <t>Estimated viscous damping of VTOL</t>
+  </si>
+  <si>
+    <t>Lh</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Nm/rad/s</t>
+  </si>
+  <si>
+    <t>Counter-weight mass</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Momenty of inertia</t>
+  </si>
+  <si>
+    <t>kgm^2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +231,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -412,11 +549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,9 +562,12 @@
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -446,8 +586,26 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>2.59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>4</v>
       </c>
@@ -468,8 +626,26 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>5.95</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>5</v>
       </c>
@@ -489,8 +665,27 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <f>K3-K2</f>
+        <v>3.3600000000000003</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4">
+        <v>0.27</v>
+      </c>
+      <c r="P4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6</v>
       </c>
@@ -507,8 +702,20 @@
       <c r="G5">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>7</v>
       </c>
@@ -528,8 +735,20 @@
       <c r="H6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6">
+        <v>15.6</v>
+      </c>
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>8</v>
       </c>
@@ -549,8 +768,20 @@
       <c r="H7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7">
+        <v>6.3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -567,9 +798,81 @@
       <c r="H8" t="s">
         <v>17</v>
       </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8">
+        <v>28.4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9">
+        <v>2E-3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>1.87</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added graph output data. Updated files
</commit_message>
<xml_diff>
--- a/Resistance and results table.xlsx
+++ b/Resistance and results table.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>Measured Current (A)</t>
   </si>
@@ -213,6 +213,24 @@
   </si>
   <si>
     <t>kgm^2</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Stiffness</t>
+  </si>
+  <si>
+    <t>(N m)/rad</t>
+  </si>
+  <si>
+    <t>Kt</t>
+  </si>
+  <si>
+    <t>Thrust_current_Torque constant</t>
+  </si>
+  <si>
+    <t>(N m)/A</t>
   </si>
 </sst>
 </file>
@@ -550,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P12"/>
+  <dimension ref="B2:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,10 +882,36 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <v>2.1850000000000001</v>
+        <v>2.6185</v>
       </c>
       <c r="H12" t="s">
         <v>24</v>
+      </c>
+      <c r="M12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>